<commit_message>
added NotAllowed Names features to robust the Extrating Names Feature
</commit_message>
<xml_diff>
--- a/Playwright/FILES/Roster_File.xlsx
+++ b/Playwright/FILES/Roster_File.xlsx
@@ -20,14 +20,14 @@
     <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'July 23 W1'!$A$1:$K$45</definedName>
     <definedName hidden="1" localSheetId="3" name="_xlnm._FilterDatabase">'July 23 W2'!$A$1:$K$42</definedName>
     <definedName hidden="1" localSheetId="4" name="_xlnm._FilterDatabase">'July 23 W3'!$A$1:$K$45</definedName>
-    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">Dashboards!$A$1:$B$33</definedName>
+    <definedName hidden="1" localSheetId="5" name="_xlnm._FilterDatabase">Dashboards!$A$1:$B$34</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="218">
   <si>
     <t>Job Title</t>
   </si>
@@ -473,7 +473,19 @@
     <t>19/07/2023</t>
   </si>
   <si>
+    <t>21/07/2023</t>
+  </si>
+  <si>
     <t>https://www.linkedin.com/jobs/view/3661981777</t>
+  </si>
+  <si>
+    <t>3D Designer</t>
+  </si>
+  <si>
+    <t>20/07/2023</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3666139558</t>
   </si>
   <si>
     <t>Business Development Officer (BDO)</t>
@@ -485,10 +497,10 @@
     <t>Al-Khobar, KSA</t>
   </si>
   <si>
-    <t>3D Designer</t>
+    <t>19/07/23</t>
   </si>
   <si>
-    <t>19/07/23</t>
+    <t>20/07/23</t>
   </si>
   <si>
     <t>https://www.linkedin.com/hiring/jobs/3668459914/detail</t>
@@ -500,16 +512,46 @@
     <t>Healthcare Program Manager</t>
   </si>
   <si>
-    <t>In review</t>
+    <t>https://www.linkedin.com/jobs/view/3665621347</t>
+  </si>
+  <si>
+    <t>in review</t>
+  </si>
+  <si>
+    <t>21/7/2023</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3671960536/</t>
   </si>
   <si>
     <t>Khilo Mal</t>
+  </si>
+  <si>
+    <t>20/7/23</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3669806530</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3668232918</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3669747100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In review </t>
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/3668425869/</t>
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/3668417786/</t>
+  </si>
+  <si>
+    <t>22/07/2023</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/jobs/view/3672253177/</t>
   </si>
   <si>
     <t>Shayan Siddiqui</t>
@@ -528,6 +570,9 @@
   </si>
   <si>
     <t>Adam Butt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New </t>
   </si>
   <si>
     <t>Ambreen Yusuf</t>
@@ -601,24 +646,8 @@
         <rFont val="Arial"/>
         <sz val="11.0"/>
       </rPr>
-      <t xml:space="preserve">Hi [Name], it seems like you still have not submitted your job application or completed your profile on your platform. Our partner [PartnerName] can only get in touch with you if they are interested in your completed profile. Adding the link again: [Job Link]
-Additionally, please make sure that your profile is up to date so that we can recommend it to our partners. Fill out all the sections to maximize your potential of getting the job. Here's the link: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <sz val="11.0"/>
-        <u/>
-      </rPr>
-      <t>https://app.qureos.com/profile.</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve"> If you need help completing the profile, check out our profile completion guide: </t>
+      <t xml:space="preserve">it seems like you still have not submitted your job application or completed your profile on your platform. Our partner  can only get in touch with you if they are interested in your completed profile.
+Additionally, please make sure that your profile is up to date so that we can recommend it to our partners. Fill out all the sections to maximize your potential of getting the job. Here's the link: https://app.qureos.com/profile. If you need help completing the profile, check out our profile completion guide: </t>
     </r>
     <r>
       <rPr>
@@ -628,13 +657,6 @@
         <u/>
       </rPr>
       <t>https://www.qureos.com/articles/qureos-profile</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="11.0"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
     </r>
   </si>
   <si>
@@ -10279,15 +10301,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="29" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
@@ -10295,36 +10317,36 @@
     </row>
     <row r="4">
       <c r="A4" s="29" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="26" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="29" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="26" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -36899,21 +36921,23 @@
       <c r="H4" s="70" t="s">
         <v>147</v>
       </c>
-      <c r="I4" s="22"/>
+      <c r="I4" s="22" t="s">
+        <v>148</v>
+      </c>
       <c r="J4" s="18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K4" s="9"/>
     </row>
     <row r="5">
-      <c r="A5" s="62" t="s">
-        <v>146</v>
+      <c r="A5" s="69" t="s">
+        <v>150</v>
       </c>
       <c r="B5" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="55" t="s">
-        <v>92</v>
+      <c r="C5" s="37" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>14</v>
@@ -36927,14 +36951,18 @@
       <c r="G5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="22" t="s">
+        <v>151</v>
+      </c>
       <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="J5" s="10" t="s">
+        <v>152</v>
+      </c>
       <c r="K5" s="9"/>
     </row>
     <row r="6">
       <c r="A6" s="75" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B6" s="55" t="s">
         <v>22</v>
@@ -36961,13 +36989,13 @@
     </row>
     <row r="7">
       <c r="A7" s="62" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B7" s="55" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="55" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
@@ -36988,7 +37016,7 @@
     </row>
     <row r="8">
       <c r="A8" s="69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="55" t="s">
         <v>22</v>
@@ -37009,11 +37037,13 @@
         <v>17</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="I8" s="13"/>
+        <v>156</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>157</v>
+      </c>
       <c r="J8" s="18" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="K8" s="9"/>
     </row>
@@ -37040,17 +37070,19 @@
         <v>17</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="I9" s="13"/>
+        <v>156</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>157</v>
+      </c>
       <c r="J9" s="18" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="K9" s="9"/>
     </row>
     <row r="10">
       <c r="A10" s="75" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B10" s="55" t="s">
         <v>22</v>
@@ -37077,7 +37109,7 @@
     </row>
     <row r="11">
       <c r="A11" s="75" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="B11" s="55" t="s">
         <v>22</v>
@@ -37101,18 +37133,20 @@
         <v>157</v>
       </c>
       <c r="I11" s="70"/>
-      <c r="J11" s="22"/>
+      <c r="J11" s="10" t="s">
+        <v>161</v>
+      </c>
       <c r="K11" s="9"/>
     </row>
     <row r="12">
       <c r="A12" s="62" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B12" s="55" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>14</v>
@@ -37126,7 +37160,9 @@
       <c r="G12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="22" t="s">
+        <v>162</v>
+      </c>
       <c r="I12" s="22"/>
       <c r="J12" s="77"/>
       <c r="K12" s="9"/>
@@ -37153,14 +37189,18 @@
       <c r="G13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="70"/>
+      <c r="H13" s="70" t="s">
+        <v>163</v>
+      </c>
       <c r="I13" s="70"/>
-      <c r="J13" s="22"/>
+      <c r="J13" s="10" t="s">
+        <v>164</v>
+      </c>
       <c r="K13" s="9"/>
     </row>
     <row r="14">
       <c r="A14" s="69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B14" s="55" t="s">
         <v>22</v>
@@ -37175,7 +37215,7 @@
         <v>15</v>
       </c>
       <c r="F14" s="79" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>17</v>
@@ -37185,7 +37225,7 @@
     </row>
     <row r="15">
       <c r="A15" s="75" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B15" s="55" t="s">
         <v>22</v>
@@ -37206,9 +37246,11 @@
         <v>17</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="J15" s="22"/>
+        <v>166</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>167</v>
+      </c>
       <c r="K15" s="22"/>
     </row>
     <row r="16">
@@ -37234,13 +37276,16 @@
         <v>17</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I16" s="40"/>
+      <c r="J16" s="60" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B17" s="55" t="s">
         <v>22</v>
@@ -37260,7 +37305,12 @@
       <c r="G17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="22"/>
+      <c r="H17" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>169</v>
+      </c>
       <c r="K17" s="22"/>
     </row>
     <row r="18">
@@ -37285,18 +37335,21 @@
       <c r="G18" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="H18" s="26" t="s">
+        <v>170</v>
+      </c>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
     </row>
     <row r="19">
       <c r="A19" s="62" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B19" s="55" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>14</v>
@@ -37313,9 +37366,11 @@
       <c r="H19" s="61" t="s">
         <v>147</v>
       </c>
-      <c r="I19" s="30"/>
+      <c r="I19" s="61" t="s">
+        <v>151</v>
+      </c>
       <c r="J19" s="60" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="K19" s="32"/>
     </row>
@@ -37344,9 +37399,11 @@
       <c r="H20" s="61" t="s">
         <v>147</v>
       </c>
-      <c r="I20" s="30"/>
+      <c r="I20" s="61" t="s">
+        <v>151</v>
+      </c>
       <c r="J20" s="72" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="K20" s="32"/>
     </row>
@@ -37372,9 +37429,13 @@
       <c r="G21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="71"/>
+      <c r="H21" s="61" t="s">
+        <v>173</v>
+      </c>
       <c r="I21" s="30"/>
-      <c r="J21" s="31"/>
+      <c r="J21" s="72" t="s">
+        <v>174</v>
+      </c>
       <c r="K21" s="32"/>
     </row>
     <row r="22">
@@ -37421,7 +37482,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>17</v>
@@ -37431,13 +37492,13 @@
     </row>
     <row r="24">
       <c r="A24" s="62" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B24" s="55" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="55" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>14</v>
@@ -37446,7 +37507,7 @@
         <v>15</v>
       </c>
       <c r="F24" s="80" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>17</v>
@@ -37471,7 +37532,7 @@
         <v>15</v>
       </c>
       <c r="F25" s="80" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>17</v>
@@ -37480,7 +37541,7 @@
         <v>147</v>
       </c>
       <c r="J25" s="26" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26">
@@ -45548,32 +45609,39 @@
     <hyperlink r:id="rId4" ref="E4"/>
     <hyperlink r:id="rId5" ref="J4"/>
     <hyperlink r:id="rId6" ref="E5"/>
-    <hyperlink r:id="rId7" ref="E6"/>
-    <hyperlink r:id="rId8" ref="E7"/>
-    <hyperlink r:id="rId9" ref="E8"/>
-    <hyperlink r:id="rId10" ref="J8"/>
-    <hyperlink r:id="rId11" ref="E9"/>
-    <hyperlink r:id="rId12" ref="J9"/>
-    <hyperlink r:id="rId13" ref="E10"/>
-    <hyperlink r:id="rId14" ref="E11"/>
-    <hyperlink r:id="rId15" ref="E12"/>
-    <hyperlink r:id="rId16" ref="E13"/>
-    <hyperlink r:id="rId17" ref="E14"/>
-    <hyperlink r:id="rId18" ref="E15"/>
-    <hyperlink r:id="rId19" ref="E16"/>
-    <hyperlink r:id="rId20" ref="E17"/>
-    <hyperlink r:id="rId21" ref="E18"/>
-    <hyperlink r:id="rId22" ref="E19"/>
-    <hyperlink r:id="rId23" ref="J19"/>
-    <hyperlink r:id="rId24" ref="E20"/>
-    <hyperlink r:id="rId25" ref="J20"/>
-    <hyperlink r:id="rId26" ref="E21"/>
-    <hyperlink r:id="rId27" ref="E22"/>
-    <hyperlink r:id="rId28" ref="E23"/>
-    <hyperlink r:id="rId29" ref="E24"/>
-    <hyperlink r:id="rId30" ref="E25"/>
+    <hyperlink r:id="rId7" ref="J5"/>
+    <hyperlink r:id="rId8" ref="E6"/>
+    <hyperlink r:id="rId9" ref="E7"/>
+    <hyperlink r:id="rId10" ref="E8"/>
+    <hyperlink r:id="rId11" ref="J8"/>
+    <hyperlink r:id="rId12" ref="E9"/>
+    <hyperlink r:id="rId13" ref="J9"/>
+    <hyperlink r:id="rId14" ref="E10"/>
+    <hyperlink r:id="rId15" ref="E11"/>
+    <hyperlink r:id="rId16" ref="J11"/>
+    <hyperlink r:id="rId17" ref="E12"/>
+    <hyperlink r:id="rId18" ref="E13"/>
+    <hyperlink r:id="rId19" ref="J13"/>
+    <hyperlink r:id="rId20" ref="E14"/>
+    <hyperlink r:id="rId21" ref="E15"/>
+    <hyperlink r:id="rId22" ref="J15"/>
+    <hyperlink r:id="rId23" ref="E16"/>
+    <hyperlink r:id="rId24" ref="J16"/>
+    <hyperlink r:id="rId25" ref="E17"/>
+    <hyperlink r:id="rId26" ref="J17"/>
+    <hyperlink r:id="rId27" ref="E18"/>
+    <hyperlink r:id="rId28" ref="E19"/>
+    <hyperlink r:id="rId29" ref="J19"/>
+    <hyperlink r:id="rId30" ref="E20"/>
+    <hyperlink r:id="rId31" ref="J20"/>
+    <hyperlink r:id="rId32" ref="E21"/>
+    <hyperlink r:id="rId33" ref="J21"/>
+    <hyperlink r:id="rId34" ref="E22"/>
+    <hyperlink r:id="rId35" ref="E23"/>
+    <hyperlink r:id="rId36" ref="E24"/>
+    <hyperlink r:id="rId37" ref="E25"/>
   </hyperlinks>
-  <drawing r:id="rId31"/>
+  <drawing r:id="rId38"/>
 </worksheet>
 </file>
 
@@ -45592,26 +45660,29 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="29" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="61" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B2" s="81" t="s">
-        <v>165</v>
+        <v>179</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="61" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4">
@@ -45619,7 +45690,7 @@
         <v>23</v>
       </c>
       <c r="B4" s="83" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5">
@@ -45627,7 +45698,7 @@
         <v>66</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6">
@@ -45635,7 +45706,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7">
@@ -45643,106 +45714,109 @@
         <v>130</v>
       </c>
       <c r="B7" s="85" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="61" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="84" t="s">
-        <v>29</v>
-      </c>
       <c r="B8" s="81" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="84" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="81" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="E9" s="86"/>
-      <c r="F9" s="87"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="88" t="s">
-        <v>38</v>
-      </c>
       <c r="B10" s="81" t="s">
-        <v>165</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="E10" s="86"/>
+      <c r="F10" s="87"/>
     </row>
     <row r="11">
       <c r="A11" s="88" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="81" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="81" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="61" t="s">
+      <c r="B12" s="81" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="B12" s="81" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="84" t="s">
+      <c r="B13" s="81" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="81" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="88" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="89"/>
-      <c r="E14" s="90"/>
+      <c r="B14" s="81" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="89"/>
+      <c r="E15" s="90"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="E15" s="90"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="61" t="s">
+      <c r="B16" s="81" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" s="90"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="E16" s="90"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="44"/>
-      <c r="B17" s="89"/>
+      <c r="B17" s="81" t="s">
+        <v>179</v>
+      </c>
       <c r="E17" s="90"/>
     </row>
     <row r="18">
-      <c r="A18" s="88"/>
-      <c r="B18" s="87"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="89"/>
       <c r="E18" s="90"/>
     </row>
     <row r="19">
+      <c r="A19" s="88"/>
       <c r="B19" s="87"/>
       <c r="E19" s="90"/>
     </row>
     <row r="20">
-      <c r="A20" s="91"/>
       <c r="B20" s="87"/>
       <c r="E20" s="90"/>
     </row>
     <row r="21">
-      <c r="A21" s="92"/>
-      <c r="B21" s="93"/>
+      <c r="A21" s="91"/>
+      <c r="B21" s="87"/>
       <c r="E21" s="90"/>
     </row>
     <row r="22">
@@ -45751,17 +45825,18 @@
       <c r="E22" s="90"/>
     </row>
     <row r="23">
-      <c r="A23" s="88"/>
-      <c r="B23" s="85"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="93"/>
       <c r="E23" s="90"/>
     </row>
     <row r="24">
-      <c r="A24" s="92"/>
-      <c r="B24" s="93"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="85"/>
+      <c r="E24" s="90"/>
     </row>
     <row r="25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="89"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="93"/>
     </row>
     <row r="26">
       <c r="A26" s="44"/>
@@ -45772,32 +45847,32 @@
       <c r="B27" s="89"/>
     </row>
     <row r="28">
-      <c r="A28" s="86"/>
+      <c r="A28" s="44"/>
       <c r="B28" s="89"/>
     </row>
     <row r="29">
-      <c r="A29" s="88"/>
-      <c r="B29" s="87"/>
+      <c r="A29" s="86"/>
+      <c r="B29" s="89"/>
     </row>
     <row r="30">
-      <c r="A30" s="44"/>
-      <c r="B30" s="89"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="87"/>
     </row>
     <row r="31">
       <c r="A31" s="44"/>
-      <c r="B31" s="93"/>
+      <c r="B31" s="89"/>
     </row>
     <row r="32">
-      <c r="A32" s="91"/>
-      <c r="B32" s="87"/>
+      <c r="A32" s="44"/>
+      <c r="B32" s="93"/>
     </row>
     <row r="33">
       <c r="A33" s="91"/>
       <c r="B33" s="87"/>
     </row>
     <row r="34">
-      <c r="A34" s="94"/>
-      <c r="B34" s="94"/>
+      <c r="A34" s="91"/>
+      <c r="B34" s="87"/>
     </row>
     <row r="35">
       <c r="A35" s="94"/>
@@ -49675,29 +49750,35 @@
       <c r="A1003" s="94"/>
       <c r="B1003" s="94"/>
     </row>
+    <row r="1004">
+      <c r="A1004" s="94"/>
+      <c r="B1004" s="94"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$B$33">
-    <sortState ref="A1:B33">
-      <sortCondition ref="A1:A33"/>
+  <autoFilter ref="$A$1:$B$34">
+    <sortState ref="A1:B34">
+      <sortCondition ref="A1:A34"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="B3"/>
-    <hyperlink r:id="rId3" ref="B4"/>
-    <hyperlink r:id="rId4" ref="B5"/>
-    <hyperlink r:id="rId5" ref="B6"/>
-    <hyperlink r:id="rId6" ref="B7"/>
-    <hyperlink r:id="rId7" ref="B8"/>
-    <hyperlink r:id="rId8" ref="B9"/>
-    <hyperlink r:id="rId9" ref="B10"/>
-    <hyperlink r:id="rId10" ref="B11"/>
-    <hyperlink r:id="rId11" ref="B12"/>
-    <hyperlink r:id="rId12" ref="B13"/>
-    <hyperlink r:id="rId13" ref="B15"/>
-    <hyperlink r:id="rId14" ref="B16"/>
+    <hyperlink r:id="rId2" ref="C2"/>
+    <hyperlink r:id="rId3" ref="B3"/>
+    <hyperlink r:id="rId4" ref="B4"/>
+    <hyperlink r:id="rId5" ref="B5"/>
+    <hyperlink r:id="rId6" ref="B6"/>
+    <hyperlink r:id="rId7" ref="B7"/>
+    <hyperlink r:id="rId8" ref="B8"/>
+    <hyperlink r:id="rId9" ref="B9"/>
+    <hyperlink r:id="rId10" ref="B10"/>
+    <hyperlink r:id="rId11" ref="B11"/>
+    <hyperlink r:id="rId12" ref="B12"/>
+    <hyperlink r:id="rId13" ref="B13"/>
+    <hyperlink r:id="rId14" ref="B14"/>
+    <hyperlink r:id="rId15" ref="B16"/>
+    <hyperlink r:id="rId16" ref="B17"/>
   </hyperlinks>
-  <drawing r:id="rId15"/>
+  <drawing r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -49720,43 +49801,43 @@
   <sheetData>
     <row r="1" ht="101.25" customHeight="1">
       <c r="A1" s="95" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="B1" s="96" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="L1" s="97"/>
     </row>
     <row r="2" ht="96.75" customHeight="1">
       <c r="A2" s="98" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" ht="114.0" customHeight="1">
       <c r="A3" s="100" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B3" s="101" t="s">
-        <v>173</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" ht="102.0" customHeight="1">
       <c r="A4" s="98" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B4" s="102" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" ht="123.75" customHeight="1">
       <c r="A5" s="100" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="B5" s="101" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6">
@@ -50180,52 +50261,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="107" t="s">
-        <v>177</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>178</v>
+        <v>193</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="107" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="B10" s="108" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="22" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="B11" s="108" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="39" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -50262,13 +50343,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="107" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="B1" s="107" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="C1" s="107" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" ht="30.0" customHeight="1">

</xml_diff>